<commit_message>
picture and spreadsheet upload
</commit_message>
<xml_diff>
--- a/spreadsheets/Elise.xlsx
+++ b/spreadsheets/Elise.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\champsgg\completed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\champsgg\completed\1_special\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370C151D-BE45-45F9-B098-03BC24CFE2AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AFA0EB-C887-43F3-B911-5F33159011D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30195" yWindow="2850" windowWidth="21525" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
   <si>
     <t>Champion</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>youtube</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>For op.gg, you can also link a multi op.gg</t>
@@ -692,7 +689,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -774,68 +771,66 @@
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>86</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>92</v>
+        <v>63</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C13" s="4"/>
     </row>
@@ -843,10 +838,10 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1834,7 +1829,7 @@
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B12" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -1951,7 +1946,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>30</v>
@@ -2019,7 +2014,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2053,18 +2048,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4">
         <v>6</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
@@ -2073,18 +2068,18 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="5">
         <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4">
         <v>2</v>
@@ -2093,18 +2088,18 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4">
         <v>8</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="4">
         <v>2</v>
@@ -2113,7 +2108,7 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4">
         <v>3</v>
@@ -2122,7 +2117,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="4">
         <v>2</v>
@@ -2131,29 +2126,29 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="4">
         <v>4</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="4">
         <v>4</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="4">
         <v>3</v>
@@ -2162,7 +2157,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="4">
         <v>3</v>
@@ -2171,7 +2166,7 @@
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="4">
         <v>2</v>
@@ -2180,7 +2175,7 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="4">
         <v>2</v>
@@ -2189,7 +2184,7 @@
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="4">
         <v>3</v>
@@ -2198,7 +2193,7 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="4">
         <v>2</v>
@@ -2207,7 +2202,7 @@
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="4">
         <v>2</v>
@@ -2216,7 +2211,7 @@
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B35" s="4">
         <v>2</v>
@@ -2225,7 +2220,7 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" s="4">
         <v>2</v>
@@ -2234,7 +2229,7 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="4">
         <v>2</v>
@@ -2243,7 +2238,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="4">
         <v>3</v>
@@ -2252,7 +2247,7 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="4">
         <v>3</v>
@@ -2261,7 +2256,7 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="4">
         <v>2</v>

</xml_diff>